<commit_message>
Commit and Push as on 07-May-2019.
</commit_message>
<xml_diff>
--- a/NwntTest/src/main/java/com/nwnt/qa/testdata/UploadReports.xlsx
+++ b/NwntTest/src/main/java/com/nwnt/qa/testdata/UploadReports.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14820" windowHeight="3840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UploadLabReports" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="RevisedMedicine" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:M11"/>
 </workbook>
 </file>
 
@@ -48,9 +49,6 @@
     <t>Haemoglobin</t>
   </si>
   <si>
-    <t>Lipid Profile</t>
-  </si>
-  <si>
     <t>Serum Lithium</t>
   </si>
   <si>
@@ -82,6 +80,9 @@
   </si>
   <si>
     <t>Decrease the sleep medicine</t>
+  </si>
+  <si>
+    <t>Lipid profile</t>
   </si>
 </sst>
 </file>
@@ -435,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -465,7 +466,7 @@
         <v>43585</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -476,40 +477,40 @@
         <v>43589</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2">
         <v>43587</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>43584</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2">
         <v>43576</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -522,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -568,7 +569,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>30</v>
@@ -579,7 +580,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>0.4</v>
@@ -590,7 +591,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>5.7</v>
@@ -628,18 +629,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>